<commit_message>
FP statuses in Area 1A
</commit_message>
<xml_diff>
--- a/data/tables/IA_BLE_Tracking.xlsx
+++ b/data/tables/IA_BLE_Tracking.xlsx
@@ -17,7 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -549,7 +553,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -557,15 +561,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2024/02/28</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2024/04/04</t>
-        </is>
+      <c r="G2" s="2" t="n">
+        <v>45350</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45386</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -590,10 +590,8 @@
       <c r="M2" t="n">
         <v>100</v>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>2024/01/10</t>
-        </is>
+      <c r="N2" s="2" t="n">
+        <v>45301</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -639,7 +637,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,15 +645,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2023/12/30</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2024/03/15</t>
-        </is>
+      <c r="G3" s="2" t="n">
+        <v>45290</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>45366</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -680,10 +674,8 @@
       <c r="M3" t="n">
         <v>100</v>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N3" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -729,7 +721,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -737,15 +729,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2024/05/22</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2024/04/15</t>
-        </is>
+      <c r="G4" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>45397</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -770,10 +758,8 @@
       <c r="M4" t="n">
         <v>100</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N4" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -819,7 +805,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -827,15 +813,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2024/05/22</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2024/05/17</t>
-        </is>
+      <c r="G5" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>45429</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -860,10 +842,8 @@
       <c r="M5" t="n">
         <v>100</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>2023/12/12</t>
-        </is>
+      <c r="N5" s="2" t="n">
+        <v>45272</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -909,7 +889,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -917,15 +897,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2024/05/22</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2024/05/09</t>
-        </is>
+      <c r="G6" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>45421</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -950,10 +926,8 @@
       <c r="M6" t="n">
         <v>100</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>2024/01/10</t>
-        </is>
+      <c r="N6" s="2" t="n">
+        <v>45301</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -999,7 +973,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1007,15 +981,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2023/11/30</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2024/02/23</t>
-        </is>
+      <c r="G7" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>45345</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -1040,10 +1010,8 @@
       <c r="M7" t="n">
         <v>100</v>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>2023/10/12</t>
-        </is>
+      <c r="N7" s="2" t="n">
+        <v>45211</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1089,7 +1057,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1097,15 +1065,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2024/01/30</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>2024/03/15</t>
-        </is>
+      <c r="G8" s="2" t="n">
+        <v>45321</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>45366</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -1130,10 +1094,8 @@
       <c r="M8" t="n">
         <v>100</v>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>2023/12/12</t>
-        </is>
+      <c r="N8" s="2" t="n">
+        <v>45272</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1179,7 +1141,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1187,15 +1149,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2024/07/13</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>2024/06/14</t>
-        </is>
+      <c r="G9" s="2" t="n">
+        <v>45486</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>45457</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1220,10 +1178,8 @@
       <c r="M9" t="n">
         <v>100</v>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>2024/05/31</t>
-        </is>
+      <c r="N9" s="2" t="n">
+        <v>45443</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1269,7 +1225,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>In Backcheck</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1277,15 +1233,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2024/03/30</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2024/04/20</t>
-        </is>
+      <c r="G10" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>45402</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1310,10 +1262,8 @@
       <c r="M10" t="n">
         <v>100</v>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>2024/02/10</t>
-        </is>
+      <c r="N10" s="2" t="n">
+        <v>45332</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1359,7 +1309,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1367,15 +1317,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2023/11/30</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2024/02/23</t>
-        </is>
+      <c r="G11" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>45345</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1400,10 +1346,8 @@
       <c r="M11" t="n">
         <v>100</v>
       </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>2023/10/12</t>
-        </is>
+      <c r="N11" s="2" t="n">
+        <v>45211</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1449,7 +1393,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1457,15 +1401,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2023/12/30</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>2024/04/15</t>
-        </is>
+      <c r="G12" s="2" t="n">
+        <v>45290</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>45397</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1490,10 +1430,8 @@
       <c r="M12" t="n">
         <v>100</v>
       </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N12" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1547,15 +1485,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2023/12/30</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>2024/03/24</t>
-        </is>
+      <c r="G13" s="2" t="n">
+        <v>45290</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>45375</v>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -1572,10 +1506,8 @@
       <c r="M13" t="n">
         <v>0</v>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N13" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1625,15 +1557,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2024/08/04</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2024/08/04</t>
-        </is>
+      <c r="G14" s="2" t="n">
+        <v>45508</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>45508</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1654,10 +1582,8 @@
       <c r="M14" t="n">
         <v>0</v>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>2024/07/25</t>
-        </is>
+      <c r="N14" s="2" t="n">
+        <v>45498</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1707,15 +1633,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2024/02/26</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>2024/02/13</t>
-        </is>
+      <c r="G15" s="2" t="n">
+        <v>45348</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>45335</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -1732,10 +1654,8 @@
       <c r="M15" t="n">
         <v>0</v>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>2023/08/12</t>
-        </is>
+      <c r="N15" s="2" t="n">
+        <v>45150</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1785,15 +1705,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2023/07/30</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>2023/08/31</t>
-        </is>
+      <c r="G16" s="2" t="n">
+        <v>45137</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>45169</v>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -1810,10 +1726,8 @@
       <c r="M16" t="n">
         <v>0</v>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>2023/06/11</t>
-        </is>
+      <c r="N16" s="2" t="n">
+        <v>45088</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1867,15 +1781,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2024/06/03</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>2024/03/05</t>
-        </is>
+      <c r="G17" s="2" t="n">
+        <v>45446</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>45356</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1896,10 +1806,8 @@
       <c r="M17" t="n">
         <v>0</v>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N17" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1949,15 +1857,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2024/02/28</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2024/03/26</t>
-        </is>
+      <c r="G18" s="2" t="n">
+        <v>45350</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>45377</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1982,10 +1886,8 @@
       <c r="M18" t="n">
         <v>0</v>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>2024/01/10</t>
-        </is>
+      <c r="N18" s="2" t="n">
+        <v>45301</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -2035,15 +1937,11 @@
           <t>In Backcheck</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2024/03/30</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2024/05/24</t>
-        </is>
+      <c r="G19" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>45436</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -2068,10 +1966,8 @@
       <c r="M19" t="n">
         <v>100</v>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>2024/02/10</t>
-        </is>
+      <c r="N19" s="2" t="n">
+        <v>45332</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -2125,15 +2021,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2024/07/30</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>2024/07/30</t>
-        </is>
+      <c r="G20" s="2" t="n">
+        <v>45503</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>45503</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -2158,10 +2050,8 @@
       <c r="M20" t="n">
         <v>100</v>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>2024/07/21</t>
-        </is>
+      <c r="N20" s="2" t="n">
+        <v>45494</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2215,15 +2105,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2024/07/11</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>2024/06/12</t>
-        </is>
+      <c r="G21" s="2" t="n">
+        <v>45484</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>45455</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -2248,10 +2134,8 @@
       <c r="M21" t="n">
         <v>100</v>
       </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>2024/07/08</t>
-        </is>
+      <c r="N21" s="2" t="n">
+        <v>45481</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2305,15 +2189,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2024/09/09</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>2024/07/12</t>
-        </is>
+      <c r="G22" s="2" t="n">
+        <v>45544</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>45485</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -2338,10 +2218,8 @@
       <c r="M22" t="n">
         <v>100</v>
       </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>2024/07/08</t>
-        </is>
+      <c r="N22" s="2" t="n">
+        <v>45481</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2395,15 +2273,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2024/08/01</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>2024/08/01</t>
-        </is>
+      <c r="G23" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>45505</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -2428,10 +2302,8 @@
       <c r="M23" t="n">
         <v>100</v>
       </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>2024/03/12</t>
-        </is>
+      <c r="N23" s="2" t="n">
+        <v>45363</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2485,15 +2357,11 @@
           <t>In Backcheck</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2024/05/29</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>2024/05/28</t>
-        </is>
+      <c r="G24" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>45440</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -2518,10 +2386,8 @@
       <c r="M24" t="n">
         <v>100</v>
       </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>2024/02/10</t>
-        </is>
+      <c r="N24" s="2" t="n">
+        <v>45332</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2575,15 +2441,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>2024/08/05</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>2024/08/06</t>
-        </is>
+      <c r="G25" s="2" t="n">
+        <v>45509</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>45510</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -2608,10 +2470,8 @@
       <c r="M25" t="n">
         <v>100</v>
       </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>2024/05/12</t>
-        </is>
+      <c r="N25" s="2" t="n">
+        <v>45424</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2665,15 +2525,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2024/08/05</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>2024/08/07</t>
-        </is>
+      <c r="G26" s="2" t="n">
+        <v>45509</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>45511</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -2698,10 +2554,8 @@
       <c r="M26" t="n">
         <v>100</v>
       </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>2024/07/16</t>
-        </is>
+      <c r="N26" s="2" t="n">
+        <v>45489</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2755,15 +2609,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2024/08/20</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>2024/08/06</t>
-        </is>
+      <c r="G27" s="2" t="n">
+        <v>45524</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>45510</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -2788,10 +2638,8 @@
       <c r="M27" t="n">
         <v>100</v>
       </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>2024/08/01</t>
-        </is>
+      <c r="N27" s="2" t="n">
+        <v>45505</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2948,7 +2796,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2956,15 +2804,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2024/02/28</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2024/04/04</t>
-        </is>
+      <c r="G2" s="2" t="n">
+        <v>45350</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45386</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -2989,10 +2833,8 @@
       <c r="M2" t="n">
         <v>100</v>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>2024/01/10</t>
-        </is>
+      <c r="N2" s="2" t="n">
+        <v>45301</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -3038,7 +2880,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -3046,15 +2888,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2023/12/30</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2024/03/15</t>
-        </is>
+      <c r="G3" s="2" t="n">
+        <v>45290</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>45366</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -3079,10 +2917,8 @@
       <c r="M3" t="n">
         <v>100</v>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N3" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -3128,7 +2964,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3136,15 +2972,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2024/05/22</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2024/04/15</t>
-        </is>
+      <c r="G4" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>45397</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -3169,10 +3001,8 @@
       <c r="M4" t="n">
         <v>100</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N4" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -3218,7 +3048,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3226,15 +3056,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2024/05/22</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2024/05/17</t>
-        </is>
+      <c r="G5" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>45429</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -3259,10 +3085,8 @@
       <c r="M5" t="n">
         <v>100</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>2023/12/12</t>
-        </is>
+      <c r="N5" s="2" t="n">
+        <v>45272</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -3308,7 +3132,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -3316,15 +3140,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2024/05/22</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2024/05/09</t>
-        </is>
+      <c r="G6" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>45421</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -3349,10 +3169,8 @@
       <c r="M6" t="n">
         <v>100</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>2024/01/10</t>
-        </is>
+      <c r="N6" s="2" t="n">
+        <v>45301</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -3398,7 +3216,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -3406,15 +3224,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2023/11/30</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2024/02/23</t>
-        </is>
+      <c r="G7" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>45345</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -3439,10 +3253,8 @@
       <c r="M7" t="n">
         <v>100</v>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>2023/10/12</t>
-        </is>
+      <c r="N7" s="2" t="n">
+        <v>45211</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -3488,7 +3300,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -3496,15 +3308,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2024/01/30</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>2024/03/15</t>
-        </is>
+      <c r="G8" s="2" t="n">
+        <v>45321</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>45366</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -3529,10 +3337,8 @@
       <c r="M8" t="n">
         <v>100</v>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>2023/12/12</t>
-        </is>
+      <c r="N8" s="2" t="n">
+        <v>45272</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -3578,7 +3384,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -3586,15 +3392,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2024/07/13</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>2024/06/14</t>
-        </is>
+      <c r="G9" s="2" t="n">
+        <v>45486</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>45457</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -3619,10 +3421,8 @@
       <c r="M9" t="n">
         <v>100</v>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>2024/05/31</t>
-        </is>
+      <c r="N9" s="2" t="n">
+        <v>45443</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -3668,7 +3468,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>In Backcheck</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -3676,15 +3476,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2024/03/30</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2024/04/20</t>
-        </is>
+      <c r="G10" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>45402</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -3709,10 +3505,8 @@
       <c r="M10" t="n">
         <v>100</v>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>2024/02/10</t>
-        </is>
+      <c r="N10" s="2" t="n">
+        <v>45332</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -3758,7 +3552,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -3766,15 +3560,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2023/11/30</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2024/02/23</t>
-        </is>
+      <c r="G11" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>45345</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -3799,10 +3589,8 @@
       <c r="M11" t="n">
         <v>100</v>
       </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>2023/10/12</t>
-        </is>
+      <c r="N11" s="2" t="n">
+        <v>45211</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -3848,7 +3636,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Submitted</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -3856,15 +3644,11 @@
           <t>Approved</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2023/12/30</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>2024/04/15</t>
-        </is>
+      <c r="G12" s="2" t="n">
+        <v>45290</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>45397</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -3889,10 +3673,8 @@
       <c r="M12" t="n">
         <v>100</v>
       </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N12" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -3946,15 +3728,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2023/12/30</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>2024/03/24</t>
-        </is>
+      <c r="G13" s="2" t="n">
+        <v>45290</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>45375</v>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -3971,10 +3749,8 @@
       <c r="M13" t="n">
         <v>0</v>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N13" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -4024,15 +3800,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2024/08/04</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2024/08/04</t>
-        </is>
+      <c r="G14" s="2" t="n">
+        <v>45508</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>45508</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -4053,10 +3825,8 @@
       <c r="M14" t="n">
         <v>0</v>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>2024/07/25</t>
-        </is>
+      <c r="N14" s="2" t="n">
+        <v>45498</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -4106,15 +3876,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2024/02/26</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>2024/02/13</t>
-        </is>
+      <c r="G15" s="2" t="n">
+        <v>45348</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>45335</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -4131,10 +3897,8 @@
       <c r="M15" t="n">
         <v>0</v>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>2023/08/12</t>
-        </is>
+      <c r="N15" s="2" t="n">
+        <v>45150</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -4184,15 +3948,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2023/07/30</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>2023/08/31</t>
-        </is>
+      <c r="G16" s="2" t="n">
+        <v>45137</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>45169</v>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
@@ -4209,10 +3969,8 @@
       <c r="M16" t="n">
         <v>0</v>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>2023/06/11</t>
-        </is>
+      <c r="N16" s="2" t="n">
+        <v>45088</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -4266,15 +4024,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2024/06/03</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>2024/03/05</t>
-        </is>
+      <c r="G17" s="2" t="n">
+        <v>45446</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>45356</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -4295,10 +4049,8 @@
       <c r="M17" t="n">
         <v>0</v>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>2023/11/11</t>
-        </is>
+      <c r="N17" s="2" t="n">
+        <v>45241</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -4348,15 +4100,11 @@
           <t>Next</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2024/02/28</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2024/03/26</t>
-        </is>
+      <c r="G18" s="2" t="n">
+        <v>45350</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>45377</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -4381,10 +4129,8 @@
       <c r="M18" t="n">
         <v>0</v>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>2024/01/10</t>
-        </is>
+      <c r="N18" s="2" t="n">
+        <v>45301</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -4434,15 +4180,11 @@
           <t>In Backcheck</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2024/03/30</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2024/05/24</t>
-        </is>
+      <c r="G19" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>45436</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -4467,10 +4209,8 @@
       <c r="M19" t="n">
         <v>100</v>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>2024/02/10</t>
-        </is>
+      <c r="N19" s="2" t="n">
+        <v>45332</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -4524,15 +4264,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2024/07/30</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>2024/07/30</t>
-        </is>
+      <c r="G20" s="2" t="n">
+        <v>45503</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>45503</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -4557,10 +4293,8 @@
       <c r="M20" t="n">
         <v>100</v>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>2024/07/21</t>
-        </is>
+      <c r="N20" s="2" t="n">
+        <v>45494</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -4614,15 +4348,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2024/07/11</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>2024/06/12</t>
-        </is>
+      <c r="G21" s="2" t="n">
+        <v>45484</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>45455</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -4647,10 +4377,8 @@
       <c r="M21" t="n">
         <v>100</v>
       </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>2024/07/08</t>
-        </is>
+      <c r="N21" s="2" t="n">
+        <v>45481</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -4704,15 +4432,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2024/09/09</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>2024/07/12</t>
-        </is>
+      <c r="G22" s="2" t="n">
+        <v>45544</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>45485</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -4737,10 +4461,8 @@
       <c r="M22" t="n">
         <v>100</v>
       </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>2024/07/08</t>
-        </is>
+      <c r="N22" s="2" t="n">
+        <v>45481</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -4794,15 +4516,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2024/08/01</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>2024/08/01</t>
-        </is>
+      <c r="G23" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>45505</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -4827,10 +4545,8 @@
       <c r="M23" t="n">
         <v>100</v>
       </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>2024/03/12</t>
-        </is>
+      <c r="N23" s="2" t="n">
+        <v>45363</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -4884,15 +4600,11 @@
           <t>In Backcheck</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2024/05/29</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>2024/05/28</t>
-        </is>
+      <c r="G24" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>45440</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -4917,10 +4629,8 @@
       <c r="M24" t="n">
         <v>100</v>
       </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>2024/02/10</t>
-        </is>
+      <c r="N24" s="2" t="n">
+        <v>45332</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -4974,15 +4684,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>2024/08/05</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>2024/08/06</t>
-        </is>
+      <c r="G25" s="2" t="n">
+        <v>45509</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>45510</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -5007,10 +4713,8 @@
       <c r="M25" t="n">
         <v>100</v>
       </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>2024/05/12</t>
-        </is>
+      <c r="N25" s="2" t="n">
+        <v>45424</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -5064,15 +4768,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2024/08/05</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>2024/08/07</t>
-        </is>
+      <c r="G26" s="2" t="n">
+        <v>45509</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>45511</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -5097,10 +4797,8 @@
       <c r="M26" t="n">
         <v>100</v>
       </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>2024/07/16</t>
-        </is>
+      <c r="N26" s="2" t="n">
+        <v>45489</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -5154,15 +4852,11 @@
           <t>Submitted</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2024/08/20</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>2024/08/06</t>
-        </is>
+      <c r="G27" s="2" t="n">
+        <v>45524</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>45510</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -5187,10 +4881,8 @@
       <c r="M27" t="n">
         <v>100</v>
       </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>2024/08/01</t>
-        </is>
+      <c r="N27" s="2" t="n">
+        <v>45505</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>

</xml_diff>